<commit_message>
nambah login site BGE, and add menu site BGE
</commit_message>
<xml_diff>
--- a/public/sampleKomputer.xlsx
+++ b/public/sampleKomputer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT PPA-BIB\Documents\PROJECT ICT SOFTWARE\IT-PORTAL-HO-FIXED-ONLY-HO\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BIB-NB-COE-034\Documents\.dafalenovo\PROJECT ICT SOFTWARE\IT-PORTAL-HO-FIXED-ONLY-HO\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CAB27BF-AAB3-482C-B855-9829D71DD9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A748BE-E7BA-4531-8234-F2D7984F9771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{AA518A1B-D065-49A0-8AFF-0FB34B05899E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AA518A1B-D065-49A0-8AFF-0FB34B05899E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="99">
   <si>
     <t>inventory_number</t>
   </si>
@@ -51,9 +51,6 @@
     <t>-</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>* PADA KOLOM STATUS HANYA BOLEH DI TULISKAN DENGAN OPSI (READY_USED, READY_STANBY, SCRAP, DAN BREAKDOWN)</t>
   </si>
   <si>
@@ -126,100 +123,205 @@
     <t>Note</t>
   </si>
   <si>
-    <t>1070xxxxxx</t>
-  </si>
-  <si>
-    <t>LENOVO</t>
-  </si>
-  <si>
-    <t>BARU</t>
-  </si>
-  <si>
-    <t>LEGION 5 PRO</t>
-  </si>
-  <si>
-    <t>Intel Core I7-14650HX</t>
-  </si>
-  <si>
     <t>500 GB</t>
   </si>
   <si>
     <t>16 GB</t>
   </si>
   <si>
-    <t>NVIDIA GEFORCE RTX 4060</t>
-  </si>
-  <si>
-    <t>SILVER</t>
-  </si>
-  <si>
-    <t>WINDOWS 11 PRO</t>
-  </si>
-  <si>
-    <t>SMP2MYECA</t>
-  </si>
-  <si>
-    <t>STANDART PROGRAM, APLIKASI ENG</t>
-  </si>
-  <si>
-    <t>OFFICE xxx</t>
-  </si>
-  <si>
-    <t>10.1.25.1</t>
-  </si>
-  <si>
-    <t>MAIN OFFICE, RUANG ENG</t>
-  </si>
-  <si>
     <t>BAGUS</t>
   </si>
   <si>
-    <t>THINKPAD X13</t>
-  </si>
-  <si>
     <t>8 GB</t>
   </si>
   <si>
-    <t>HITAM</t>
-  </si>
-  <si>
-    <t>SMP2MYECB</t>
-  </si>
-  <si>
     <t>STANDART PROGRAM, APLIKASI PLANT</t>
   </si>
   <si>
-    <t>10.1.25.2</t>
-  </si>
-  <si>
-    <t>OFFICE PLANT</t>
-  </si>
-  <si>
-    <t>LAMA</t>
-  </si>
-  <si>
     <t>1 TB</t>
   </si>
   <si>
-    <t>WINDOWS 10 HOME</t>
-  </si>
-  <si>
-    <t>SMP2MYECC</t>
-  </si>
-  <si>
     <t>STANDART PROGRAM</t>
   </si>
   <si>
-    <t>10.1.25.3</t>
-  </si>
-  <si>
-    <t>HO-PC-COE-001</t>
-  </si>
-  <si>
-    <t>HO-PC-COE-002</t>
-  </si>
-  <si>
-    <t>HO-PC-COE-003</t>
+    <t>SKS-PC-COE-001</t>
+  </si>
+  <si>
+    <t>Lenovo</t>
+  </si>
+  <si>
+    <t>standart</t>
+  </si>
+  <si>
+    <t>Thinkcentre Neo 50T</t>
+  </si>
+  <si>
+    <t>Intel Core i5 12400</t>
+  </si>
+  <si>
+    <t>INTEL INSIDE</t>
+  </si>
+  <si>
+    <t>Hitam</t>
+  </si>
+  <si>
+    <t>WIN 11 Original</t>
+  </si>
+  <si>
+    <t>GM045AEZ</t>
+  </si>
+  <si>
+    <t>MAIN OFFICE</t>
+  </si>
+  <si>
+    <t>SKS-PC-COE-002</t>
+  </si>
+  <si>
+    <t>Intel</t>
+  </si>
+  <si>
+    <t>non_standart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intel </t>
+  </si>
+  <si>
+    <t>Intel Core i7 7700</t>
+  </si>
+  <si>
+    <t>Geforce Rtx</t>
+  </si>
+  <si>
+    <t>MAIN OFFICE, RUANG COE</t>
+  </si>
+  <si>
+    <t>SKS-PC-COE-003</t>
+  </si>
+  <si>
+    <t>Intel Core i7 10700</t>
+  </si>
+  <si>
+    <t>SKS-PC-SCM-004</t>
+  </si>
+  <si>
+    <t>GM0453KH</t>
+  </si>
+  <si>
+    <t>WAREHOUSE</t>
+  </si>
+  <si>
+    <t>SKS-PC-FIN-001</t>
+  </si>
+  <si>
+    <t>Sub-con</t>
+  </si>
+  <si>
+    <t>SKS-PC-SCM-005</t>
+  </si>
+  <si>
+    <t>SKS-PC-SCM-001</t>
+  </si>
+  <si>
+    <t>GM06A692</t>
+  </si>
+  <si>
+    <t>SKS-PC-SCM-003</t>
+  </si>
+  <si>
+    <t>GM06A681</t>
+  </si>
+  <si>
+    <t>SKS-PC-PLT-003</t>
+  </si>
+  <si>
+    <t>Intel Core i5 12399</t>
+  </si>
+  <si>
+    <t>GM06A67F</t>
+  </si>
+  <si>
+    <t>WORKSHOP</t>
+  </si>
+  <si>
+    <t>SKS-PC-PLT-001</t>
+  </si>
+  <si>
+    <t>GM06A68G</t>
+  </si>
+  <si>
+    <t>SKS-PC-PLT-004</t>
+  </si>
+  <si>
+    <t>GM06A69G</t>
+  </si>
+  <si>
+    <t>SKS-PC-PLT-002</t>
+  </si>
+  <si>
+    <t>M70A</t>
+  </si>
+  <si>
+    <t>Intel Core i5</t>
+  </si>
+  <si>
+    <t>PC27VAFO</t>
+  </si>
+  <si>
+    <t>SKS-PC-PRD-001</t>
+  </si>
+  <si>
+    <t>NUC</t>
+  </si>
+  <si>
+    <t>Intel Core i3</t>
+  </si>
+  <si>
+    <t>WIN 10 Original</t>
+  </si>
+  <si>
+    <t>G6BE909006SO</t>
+  </si>
+  <si>
+    <t>PIT TAMBANG, RUANG CMC</t>
+  </si>
+  <si>
+    <t>SKS-PC-PRD-002</t>
+  </si>
+  <si>
+    <t>G6BE909006PV</t>
+  </si>
+  <si>
+    <t>SKS-PC-SHE-001</t>
+  </si>
+  <si>
+    <t>GM06A68D</t>
+  </si>
+  <si>
+    <t>MAIN OFFICE, RUANG MEDIC</t>
+  </si>
+  <si>
+    <t>SKS-PC-SHE-002</t>
+  </si>
+  <si>
+    <t>Intel Core i5 12401</t>
+  </si>
+  <si>
+    <t>GM0GAGA7</t>
+  </si>
+  <si>
+    <t>MAIN OFFICE, RUANG SHE</t>
+  </si>
+  <si>
+    <t>SKS-PC-SHE-003</t>
+  </si>
+  <si>
+    <t>G6BE92400LGH</t>
+  </si>
+  <si>
+    <t>STANDART PROGRAM, APLIKASI SHE</t>
+  </si>
+  <si>
+    <t>MAIN OFFICE, RUANG CUTTING</t>
   </si>
 </sst>
 </file>
@@ -396,18 +498,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -422,6 +512,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -759,71 +861,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C41EB6C-1614-4483-BF76-7A2D3A426679}">
-  <dimension ref="A1:V31"/>
+  <dimension ref="A1:V33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A17" sqref="A17:V33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.7265625" customWidth="1"/>
-    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.36328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.36328125" customWidth="1"/>
-    <col min="7" max="7" width="34.36328125" customWidth="1"/>
-    <col min="8" max="8" width="14.90625" customWidth="1"/>
-    <col min="9" max="9" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="34.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="28" customWidth="1"/>
-    <col min="11" max="11" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30.1796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="33.6328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-    </row>
-    <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-    </row>
-    <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+    </row>
+    <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+    </row>
+    <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -841,7 +943,7 @@
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
     </row>
-    <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -859,9 +961,9 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="3"/>
@@ -877,9 +979,9 @@
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
     </row>
-    <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -895,9 +997,9 @@
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
     </row>
-    <row r="7" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -913,9 +1015,9 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="3"/>
@@ -931,7 +1033,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -947,7 +1049,7 @@
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
     </row>
-    <row r="10" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -963,7 +1065,7 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="3"/>
@@ -979,41 +1081,41 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-    </row>
-    <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-    </row>
-    <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+    </row>
+    <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+    </row>
+    <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="3"/>
@@ -1029,7 +1131,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -1045,193 +1147,189 @@
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
     </row>
-    <row r="16" spans="1:22" ht="37.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="12" t="s">
+    <row r="16" spans="1:22" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="F16" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="G16" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="H16" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="I16" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I16" s="13" t="s">
+      <c r="J16" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="J16" s="13" t="s">
+      <c r="K16" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="K16" s="13" t="s">
+      <c r="L16" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="13" t="s">
+      <c r="M16" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="M16" s="13" t="s">
+      <c r="N16" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="N16" s="14" t="s">
+      <c r="O16" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="O16" s="14" t="s">
+      <c r="P16" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="P16" s="14" t="s">
+      <c r="Q16" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="Q16" s="14" t="s">
+      <c r="R16" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="R16" s="14" t="s">
+      <c r="S16" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="S16" s="14" t="s">
+      <c r="T16" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="T16" s="14" t="s">
+      <c r="U16" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="U16" s="15" t="s">
+      <c r="V16" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="V16" s="14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>1</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="12">
+        <v>107005899</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I17" s="1" t="s">
+      <c r="K17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="P17" s="1" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="S17" s="1" t="s">
         <v>1</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="U17" s="1">
-        <v>22003193</v>
+        <v>24001338</v>
       </c>
       <c r="V17" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>2</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I18" s="1" t="s">
+      <c r="K18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="P18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="R18" s="1" t="s">
         <v>55</v>
@@ -1240,86 +1338,983 @@
         <v>1</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="U18" s="1">
-        <v>22003193</v>
+        <v>16041185</v>
       </c>
       <c r="V18" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>3</v>
       </c>
-      <c r="B19" s="16" t="s">
-        <v>33</v>
+      <c r="B19" s="12" t="s">
+        <v>7</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="G19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="J19" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>7</v>
+        <v>54</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="P19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="S19" s="1" t="s">
         <v>1</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="U19" s="1">
-        <v>22003193</v>
+        <v>16041185</v>
       </c>
       <c r="V19" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>107005829</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" t="s">
+        <v>43</v>
+      </c>
+      <c r="H20" t="s">
+        <v>37</v>
+      </c>
+      <c r="J20" t="s">
+        <v>33</v>
+      </c>
+      <c r="K20" t="s">
+        <v>44</v>
+      </c>
+      <c r="L20" t="s">
+        <v>45</v>
+      </c>
+      <c r="M20" t="s">
+        <v>46</v>
+      </c>
+      <c r="N20" t="s">
+        <v>59</v>
+      </c>
+      <c r="O20" t="s">
+        <v>38</v>
+      </c>
+      <c r="P20" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>7</v>
+      </c>
+      <c r="R20" t="s">
+        <v>60</v>
+      </c>
+      <c r="S20" t="s">
+        <v>1</v>
+      </c>
+      <c r="T20" t="s">
+        <v>34</v>
+      </c>
+      <c r="U20">
+        <v>17102835</v>
+      </c>
+      <c r="V20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>107005830</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" t="s">
+        <v>43</v>
+      </c>
+      <c r="H21" t="s">
+        <v>37</v>
+      </c>
+      <c r="J21" t="s">
+        <v>33</v>
+      </c>
+      <c r="K21" t="s">
+        <v>44</v>
+      </c>
+      <c r="L21" t="s">
+        <v>45</v>
+      </c>
+      <c r="M21" t="s">
+        <v>46</v>
+      </c>
+      <c r="N21" t="s">
+        <v>47</v>
+      </c>
+      <c r="O21" t="s">
+        <v>38</v>
+      </c>
+      <c r="P21" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>7</v>
+      </c>
+      <c r="R21" t="s">
+        <v>60</v>
+      </c>
+      <c r="S21" t="s">
+        <v>1</v>
+      </c>
+      <c r="T21" t="s">
+        <v>34</v>
+      </c>
+      <c r="U21">
+        <v>210916055</v>
+      </c>
+      <c r="V21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <v>107006079</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" t="s">
+        <v>43</v>
+      </c>
+      <c r="H22" t="s">
+        <v>37</v>
+      </c>
+      <c r="J22" t="s">
+        <v>33</v>
+      </c>
+      <c r="K22" t="s">
+        <v>44</v>
+      </c>
+      <c r="L22" t="s">
+        <v>45</v>
+      </c>
+      <c r="M22" t="s">
+        <v>46</v>
+      </c>
+      <c r="N22" t="s">
+        <v>7</v>
+      </c>
+      <c r="O22" t="s">
+        <v>38</v>
+      </c>
+      <c r="P22" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>7</v>
+      </c>
+      <c r="R22" t="s">
+        <v>60</v>
+      </c>
+      <c r="S22" t="s">
+        <v>1</v>
+      </c>
+      <c r="T22" t="s">
+        <v>34</v>
+      </c>
+      <c r="U22">
+        <v>15111141</v>
+      </c>
+      <c r="V22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>7</v>
+      </c>
+      <c r="B23">
+        <v>107006369</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" t="s">
+        <v>43</v>
+      </c>
+      <c r="H23" t="s">
+        <v>37</v>
+      </c>
+      <c r="J23" t="s">
+        <v>33</v>
+      </c>
+      <c r="K23" t="s">
+        <v>44</v>
+      </c>
+      <c r="L23" t="s">
+        <v>45</v>
+      </c>
+      <c r="M23" t="s">
+        <v>46</v>
+      </c>
+      <c r="N23" t="s">
+        <v>65</v>
+      </c>
+      <c r="O23" t="s">
+        <v>38</v>
+      </c>
+      <c r="P23" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>7</v>
+      </c>
+      <c r="R23" t="s">
+        <v>60</v>
+      </c>
+      <c r="S23" t="s">
+        <v>1</v>
+      </c>
+      <c r="T23" t="s">
+        <v>34</v>
+      </c>
+      <c r="U23">
+        <v>21000782</v>
+      </c>
+      <c r="V23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>107006368</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" t="s">
+        <v>43</v>
+      </c>
+      <c r="H24" t="s">
+        <v>37</v>
+      </c>
+      <c r="J24" t="s">
+        <v>33</v>
+      </c>
+      <c r="K24" t="s">
+        <v>44</v>
+      </c>
+      <c r="L24" t="s">
+        <v>45</v>
+      </c>
+      <c r="M24" t="s">
+        <v>46</v>
+      </c>
+      <c r="N24" t="s">
+        <v>67</v>
+      </c>
+      <c r="O24" t="s">
+        <v>38</v>
+      </c>
+      <c r="P24" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>7</v>
+      </c>
+      <c r="R24" t="s">
+        <v>60</v>
+      </c>
+      <c r="S24" t="s">
+        <v>1</v>
+      </c>
+      <c r="T24" t="s">
+        <v>34</v>
+      </c>
+      <c r="U24">
+        <v>23002050</v>
+      </c>
+      <c r="V24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>9</v>
+      </c>
+      <c r="B25">
+        <v>107006007</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25" t="s">
+        <v>69</v>
+      </c>
+      <c r="I25" t="s">
+        <v>37</v>
+      </c>
+      <c r="J25" t="s">
+        <v>33</v>
+      </c>
+      <c r="K25" t="s">
+        <v>44</v>
+      </c>
+      <c r="L25" t="s">
+        <v>45</v>
+      </c>
+      <c r="M25" t="s">
+        <v>46</v>
+      </c>
+      <c r="N25" t="s">
+        <v>70</v>
+      </c>
+      <c r="O25" t="s">
+        <v>38</v>
+      </c>
+      <c r="P25" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>7</v>
+      </c>
+      <c r="R25" t="s">
+        <v>71</v>
+      </c>
+      <c r="S25" t="s">
+        <v>1</v>
+      </c>
+      <c r="T25" t="s">
+        <v>34</v>
+      </c>
+      <c r="U25">
+        <v>17021869</v>
+      </c>
+      <c r="V25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>10</v>
+      </c>
+      <c r="B26">
+        <v>107006366</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" t="s">
+        <v>43</v>
+      </c>
+      <c r="H26" t="s">
+        <v>37</v>
+      </c>
+      <c r="J26" t="s">
+        <v>33</v>
+      </c>
+      <c r="K26" t="s">
+        <v>44</v>
+      </c>
+      <c r="L26" t="s">
+        <v>45</v>
+      </c>
+      <c r="M26" t="s">
+        <v>46</v>
+      </c>
+      <c r="N26" t="s">
+        <v>73</v>
+      </c>
+      <c r="O26" t="s">
+        <v>38</v>
+      </c>
+      <c r="P26" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>7</v>
+      </c>
+      <c r="R26" t="s">
+        <v>71</v>
+      </c>
+      <c r="S26" t="s">
+        <v>1</v>
+      </c>
+      <c r="T26" t="s">
+        <v>34</v>
+      </c>
+      <c r="U26">
+        <v>17021869</v>
+      </c>
+      <c r="V26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>11</v>
+      </c>
+      <c r="B27">
+        <v>107006367</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27" t="s">
+        <v>42</v>
+      </c>
+      <c r="G27" t="s">
+        <v>43</v>
+      </c>
+      <c r="H27" t="s">
+        <v>37</v>
+      </c>
+      <c r="J27" t="s">
+        <v>33</v>
+      </c>
+      <c r="K27" t="s">
+        <v>44</v>
+      </c>
+      <c r="L27" t="s">
+        <v>45</v>
+      </c>
+      <c r="M27" t="s">
+        <v>46</v>
+      </c>
+      <c r="N27" t="s">
+        <v>75</v>
+      </c>
+      <c r="O27" t="s">
+        <v>38</v>
+      </c>
+      <c r="P27" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>7</v>
+      </c>
+      <c r="R27" t="s">
+        <v>71</v>
+      </c>
+      <c r="S27" t="s">
+        <v>1</v>
+      </c>
+      <c r="T27" t="s">
+        <v>34</v>
+      </c>
+      <c r="U27">
+        <v>17021869</v>
+      </c>
+      <c r="V27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>12</v>
+      </c>
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" t="s">
+        <v>51</v>
+      </c>
+      <c r="F28" t="s">
+        <v>77</v>
+      </c>
+      <c r="G28" t="s">
+        <v>78</v>
+      </c>
+      <c r="H28" t="s">
+        <v>37</v>
+      </c>
+      <c r="J28" t="s">
+        <v>35</v>
+      </c>
+      <c r="K28" t="s">
+        <v>44</v>
+      </c>
+      <c r="L28" t="s">
+        <v>45</v>
+      </c>
+      <c r="M28" t="s">
+        <v>46</v>
+      </c>
+      <c r="N28" t="s">
+        <v>79</v>
+      </c>
+      <c r="O28" t="s">
+        <v>36</v>
+      </c>
+      <c r="P28" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>7</v>
+      </c>
+      <c r="R28" t="s">
+        <v>71</v>
+      </c>
+      <c r="S28" t="s">
+        <v>1</v>
+      </c>
+      <c r="T28" t="s">
+        <v>34</v>
+      </c>
+      <c r="U28">
+        <v>17021869</v>
+      </c>
+      <c r="V28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>13</v>
+      </c>
+      <c r="B29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29" t="s">
+        <v>81</v>
+      </c>
+      <c r="G29" t="s">
+        <v>82</v>
+      </c>
+      <c r="I29" t="s">
+        <v>32</v>
+      </c>
+      <c r="J29" t="s">
+        <v>35</v>
+      </c>
+      <c r="K29" t="s">
+        <v>44</v>
+      </c>
+      <c r="L29" t="s">
+        <v>45</v>
+      </c>
+      <c r="M29" t="s">
+        <v>83</v>
+      </c>
+      <c r="N29" t="s">
+        <v>84</v>
+      </c>
+      <c r="O29" t="s">
+        <v>38</v>
+      </c>
+      <c r="P29" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>7</v>
+      </c>
+      <c r="R29" t="s">
+        <v>85</v>
+      </c>
+      <c r="S29" t="s">
+        <v>1</v>
+      </c>
+      <c r="T29" t="s">
+        <v>34</v>
+      </c>
+      <c r="U29">
+        <v>17112936</v>
+      </c>
+      <c r="V29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>14</v>
+      </c>
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D30" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" t="s">
+        <v>51</v>
+      </c>
+      <c r="F30" t="s">
+        <v>81</v>
+      </c>
+      <c r="G30" t="s">
+        <v>82</v>
+      </c>
+      <c r="I30" t="s">
+        <v>32</v>
+      </c>
+      <c r="J30" t="s">
+        <v>35</v>
+      </c>
+      <c r="K30" t="s">
+        <v>44</v>
+      </c>
+      <c r="L30" t="s">
+        <v>45</v>
+      </c>
+      <c r="M30" t="s">
+        <v>83</v>
+      </c>
+      <c r="N30" t="s">
+        <v>87</v>
+      </c>
+      <c r="O30" t="s">
+        <v>38</v>
+      </c>
+      <c r="P30" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>7</v>
+      </c>
+      <c r="R30" t="s">
+        <v>85</v>
+      </c>
+      <c r="S30" t="s">
+        <v>1</v>
+      </c>
+      <c r="T30" t="s">
+        <v>34</v>
+      </c>
+      <c r="U30">
+        <v>17112936</v>
+      </c>
+      <c r="V30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>15</v>
+      </c>
+      <c r="B31">
+        <v>107006268</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="D31" t="s">
-        <v>8</v>
+        <v>40</v>
+      </c>
+      <c r="E31" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G31" t="s">
+        <v>43</v>
+      </c>
+      <c r="I31" t="s">
+        <v>37</v>
+      </c>
+      <c r="J31" t="s">
+        <v>33</v>
+      </c>
+      <c r="K31" t="s">
+        <v>44</v>
+      </c>
+      <c r="L31" t="s">
+        <v>45</v>
+      </c>
+      <c r="M31" t="s">
+        <v>46</v>
+      </c>
+      <c r="N31" t="s">
+        <v>89</v>
+      </c>
+      <c r="O31" t="s">
+        <v>38</v>
+      </c>
+      <c r="P31" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>7</v>
+      </c>
+      <c r="R31" t="s">
+        <v>90</v>
+      </c>
+      <c r="S31" t="s">
+        <v>1</v>
+      </c>
+      <c r="T31" t="s">
+        <v>34</v>
+      </c>
+      <c r="U31">
+        <v>21000827</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>16</v>
+      </c>
+      <c r="B32">
+        <v>107006006</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32" t="s">
+        <v>41</v>
+      </c>
+      <c r="F32" t="s">
+        <v>42</v>
+      </c>
+      <c r="G32" t="s">
+        <v>92</v>
+      </c>
+      <c r="I32" t="s">
+        <v>37</v>
+      </c>
+      <c r="J32" t="s">
+        <v>33</v>
+      </c>
+      <c r="K32" t="s">
+        <v>44</v>
+      </c>
+      <c r="L32" t="s">
+        <v>45</v>
+      </c>
+      <c r="M32" t="s">
+        <v>46</v>
+      </c>
+      <c r="N32" t="s">
+        <v>93</v>
+      </c>
+      <c r="O32" t="s">
+        <v>38</v>
+      </c>
+      <c r="P32" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>7</v>
+      </c>
+      <c r="R32" t="s">
+        <v>94</v>
+      </c>
+      <c r="S32" t="s">
+        <v>1</v>
+      </c>
+      <c r="T32" t="s">
+        <v>34</v>
+      </c>
+      <c r="U32">
+        <v>22001998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>17</v>
+      </c>
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D33" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" t="s">
+        <v>51</v>
+      </c>
+      <c r="F33" t="s">
+        <v>81</v>
+      </c>
+      <c r="G33" t="s">
+        <v>82</v>
+      </c>
+      <c r="H33" t="s">
+        <v>37</v>
+      </c>
+      <c r="J33" t="s">
+        <v>35</v>
+      </c>
+      <c r="K33" t="s">
+        <v>44</v>
+      </c>
+      <c r="L33" t="s">
+        <v>45</v>
+      </c>
+      <c r="M33" t="s">
+        <v>83</v>
+      </c>
+      <c r="N33" t="s">
+        <v>96</v>
+      </c>
+      <c r="O33" t="s">
+        <v>97</v>
+      </c>
+      <c r="P33" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>7</v>
+      </c>
+      <c r="R33" t="s">
+        <v>98</v>
+      </c>
+      <c r="S33" t="s">
+        <v>1</v>
+      </c>
+      <c r="T33" t="s">
+        <v>34</v>
+      </c>
+      <c r="U33">
+        <v>210916022</v>
+      </c>
+      <c r="V33" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>